<commit_message>
Lab 12 and previous refactoring
</commit_message>
<xml_diff>
--- a/Tasks/LabTest3/Operation Count.xlsx
+++ b/Tasks/LabTest3/Operation Count.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="P:\TEMP\CoreProgramming\CProjects\DataStructuresCourse\Tasks\LabTest3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF3D8F7E-A8A2-45E7-A566-497EBCC5C86B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF48CF90-F9E4-4423-8829-6C0FB681FC6A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{691A4EAC-BEF8-4855-9107-E54E383D194B}"/>
   </bookViews>
@@ -136,7 +136,7 @@
     <c:plotArea>
       <c:layout/>
       <c:scatterChart>
-        <c:scatterStyle val="lineMarker"/>
+        <c:scatterStyle val="smoothMarker"/>
         <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
@@ -151,26 +151,14 @@
             <a:effectLst/>
           </c:spPr>
           <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="5"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent1"/>
-              </a:solidFill>
-              <a:ln w="9525">
-                <a:solidFill>
-                  <a:schemeClr val="accent1"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
+            <c:symbol val="none"/>
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$A$3:$A$11</c:f>
+              <c:f>Sheet1!$A$3:$A$12</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="9"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>100000</c:v>
                 </c:pt>
@@ -197,16 +185,19 @@
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>900000</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1000000</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$B$3:$B$11</c:f>
+              <c:f>Sheet1!$B$3:$B$12</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="9"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>12</c:v>
                 </c:pt>
@@ -233,14 +224,17 @@
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>18</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
-          <c:smooth val="0"/>
+          <c:smooth val="1"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-3BB0-4673-AD93-0C9F8252EA37}"/>
+              <c16:uniqueId val="{00000000-2C55-4D5E-B80A-0C99923ECD6A}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -252,11 +246,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="487900208"/>
-        <c:axId val="487896272"/>
+        <c:axId val="1105381695"/>
+        <c:axId val="1105381279"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="487900208"/>
+        <c:axId val="1105381695"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -313,12 +307,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="487896272"/>
+        <c:crossAx val="1105381279"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="487896272"/>
+        <c:axId val="1105381279"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -375,7 +369,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="487900208"/>
+        <c:crossAx val="1105381695"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -389,6 +383,13 @@
     </c:plotArea>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
     <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
@@ -984,23 +985,23 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>388620</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>95250</xdr:rowOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>195262</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>80962</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>83820</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>95250</xdr:rowOff>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>500062</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>157162</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="5" name="Chart 4">
+        <xdr:cNvPr id="6" name="Chart 5">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F2EC835A-260B-4FC0-BAAA-811A35370298}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E0DF14DA-CB61-469E-9D75-6C7D4B9D97E8}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1321,7 +1322,7 @@
   <dimension ref="A1:B12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="P10" sqref="P10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>